<commit_message>
Proof of concept complete
It's working!
</commit_message>
<xml_diff>
--- a/Resources/Lists.xlsx
+++ b/Resources/Lists.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12855"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="28755" windowHeight="12855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Afflictions" sheetId="1" r:id="rId1"/>
     <sheet name="Fruit" sheetId="2" r:id="rId2"/>
     <sheet name="Veg" sheetId="3" r:id="rId3"/>
-    <sheet name="Surnames" sheetId="4" r:id="rId4"/>
+    <sheet name="Prez" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="183">
   <si>
     <t>Sceptic</t>
   </si>
@@ -449,6 +449,123 @@
   </si>
   <si>
     <t>Watercress</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Jefferson</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Monroe</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Harrison</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>Polk</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Fillmore</t>
+  </si>
+  <si>
+    <t>Pierce</t>
+  </si>
+  <si>
+    <t>Buchanan</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Hayes</t>
+  </si>
+  <si>
+    <t>Garfield</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>McKinley</t>
+  </si>
+  <si>
+    <t>Roosevelt</t>
+  </si>
+  <si>
+    <t>Taft</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Harding</t>
+  </si>
+  <si>
+    <t>Coolidge</t>
+  </si>
+  <si>
+    <t>Hoover</t>
+  </si>
+  <si>
+    <t>Truman</t>
+  </si>
+  <si>
+    <t>Eisenhower</t>
+  </si>
+  <si>
+    <t>Kennedy</t>
+  </si>
+  <si>
+    <t>Nixon</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>Reagan</t>
+  </si>
+  <si>
+    <t>Bush</t>
+  </si>
+  <si>
+    <t>Clinton</t>
+  </si>
+  <si>
+    <t>Obama</t>
+  </si>
+  <si>
+    <t>Trump</t>
+  </si>
+  <si>
+    <t>Van Buren</t>
   </si>
 </sst>
 </file>
@@ -782,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B63"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2098,12 +2215,422 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="str">
+        <f t="shared" ref="B1:B45" si="0">""""&amp;A1&amp;""","</f>
+        <v>"Washington",</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" si="0"/>
+        <v>"Adams",</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>"Jefferson",</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Madison",</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Monroe",</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Adams",</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Jackson",</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Van Buren",</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Harrison",</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Tyler",</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Polk",</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Taylor",</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Fillmore",</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pierce",</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Buchanan",</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Lincoln",</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Johnson",</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Grant",</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>"Hayes",</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Garfield",</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Arthur",</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cleveland",</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Harrison",</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cleveland",</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>"McKinley",</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>"Roosevelt",</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>"Taft",</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Wilson",</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Harding",</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Coolidge",</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>"Hoover",</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>"Roosevelt",</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>"Truman",</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>"Eisenhower",</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>"Kennedy",</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>"Johnson",</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>174</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>"Nixon",</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>"Ford",</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>176</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>"Carter",</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>"Reagan",</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bush",</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>179</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>"Clinton",</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>178</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bush",</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>180</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>"Obama",</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>"Trump",</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>